<commit_message>
Fixing Bulk Operation Template
</commit_message>
<xml_diff>
--- a/LinoVative.Web.Api/Resources/ExcelFiles/CreateItemCategoryTemplate.xlsx
+++ b/LinoVative.Web.Api/Resources/ExcelFiles/CreateItemCategoryTemplate.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\LINOVATIVE\LinoVativeProject\LinovativeSolution\Linovative.Api\Resources\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\LinoValtiveSolutions\LinoVative.Web.Api\Resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164B6426-E2C0-4F8A-8A57-35DEFA36D2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D1AEB6-399D-4EB1-B1C9-DB1E8F4BD38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11085" yWindow="-32520" windowWidth="57840" windowHeight="31920" xr2:uid="{DDEE30A6-2B18-41C6-85EB-1999D5C66F47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{DDEE30A6-2B18-41C6-85EB-1999D5C66F47}"/>
   </bookViews>
   <sheets>
-    <sheet name="Create Item Category" sheetId="1" r:id="rId1"/>
+    <sheet name="Create Category" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -427,17 +427,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56733355-42C7-4069-9CC5-8A34B990EF30}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Fixing get template for bulk operation
</commit_message>
<xml_diff>
--- a/LinoVative.Web.Api/Resources/ExcelFiles/CreateItemCategoryTemplate.xlsx
+++ b/LinoVative.Web.Api/Resources/ExcelFiles/CreateItemCategoryTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\LinoValtiveSolutions\LinoVative.Web.Api\Resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D1AEB6-399D-4EB1-B1C9-DB1E8F4BD38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B18682-53FC-448D-9D7A-A57BDB653509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{DDEE30A6-2B18-41C6-85EB-1999D5C66F47}"/>
   </bookViews>
@@ -55,6 +55,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="2" tint="-0.749992370372631"/>
       <name val="Aptos Narrow"/>
@@ -427,7 +428,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56733355-42C7-4069-9CC5-8A34B990EF30}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Download Error Records API
</commit_message>
<xml_diff>
--- a/LinoVative.Web.Api/Resources/ExcelFiles/CreateItemCategoryTemplate.xlsx
+++ b/LinoVative.Web.Api/Resources/ExcelFiles/CreateItemCategoryTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\LinoValtiveSolutions\LinoVative.Web.Api\Resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B18682-53FC-448D-9D7A-A57BDB653509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246BA162-9827-4663-BCF9-7B4766A6DA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{DDEE30A6-2B18-41C6-85EB-1999D5C66F47}"/>
   </bookViews>
@@ -34,12 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Item Category Name</t>
+    <t>ID</t>
   </si>
   <si>
-    <t>Item Group Name</t>
+    <t>Category Name</t>
+  </si>
+  <si>
+    <t>Group Name</t>
   </si>
 </sst>
 </file>
@@ -426,24 +429,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56733355-42C7-4069-9CC5-8A34B990EF30}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47" customWidth="1"/>
-    <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="47" customWidth="1"/>
+    <col min="3" max="3" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>